<commit_message>
Mejora de la interfaz y correcion de erroes.
</commit_message>
<xml_diff>
--- a/docs/datos_70_registros.xlsx
+++ b/docs/datos_70_registros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epnecuador-my.sharepoint.com/personal/alexis_lapo_epn_edu_ec/Documents/Cositas/WordExcel/generador_documentos/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_FFC65FC0E1316FFDAE160BAA73CA77184180DC19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E66B30D-D0E2-4155-990E-BC4D0DDBF61F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_FFC65FC0E1316FFDAE160BAA73CA77184180DC19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A47EEB-443E-40B6-A5B6-7587EE17E10F}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9528" yWindow="1764" windowWidth="8844" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -717,11 +717,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,6 +741,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,18 +1036,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="36.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1050,7 +1060,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C2" t="s">
@@ -1061,7 +1071,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C3" t="s">
@@ -1072,7 +1082,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C4" t="s">
@@ -1083,7 +1093,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C5" t="s">
@@ -1094,7 +1104,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C6" t="s">
@@ -1105,7 +1115,7 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C7" t="s">
@@ -1116,7 +1126,7 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C8" t="s">
@@ -1127,7 +1137,7 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C9" t="s">
@@ -1138,7 +1148,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C10" t="s">
@@ -1149,7 +1159,7 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C11" t="s">
@@ -1160,7 +1170,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C12" t="s">
@@ -1171,7 +1181,7 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C13" t="s">
@@ -1182,7 +1192,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C14" t="s">
@@ -1193,7 +1203,7 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C15" t="s">
@@ -1204,7 +1214,7 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C16" t="s">
@@ -1215,7 +1225,7 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C17" t="s">
@@ -1226,7 +1236,7 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C18" t="s">
@@ -1237,7 +1247,7 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C19" t="s">
@@ -1248,7 +1258,7 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C20" t="s">
@@ -1259,7 +1269,7 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C21" t="s">
@@ -1270,7 +1280,7 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C22" t="s">
@@ -1281,7 +1291,7 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C23" t="s">
@@ -1292,7 +1302,7 @@
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C24" t="s">
@@ -1303,7 +1313,7 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C25" t="s">
@@ -1314,7 +1324,7 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C26" t="s">
@@ -1325,7 +1335,7 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C27" t="s">
@@ -1336,7 +1346,7 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C28" t="s">
@@ -1347,7 +1357,7 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C29" t="s">
@@ -1358,7 +1368,7 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C30" t="s">
@@ -1369,7 +1379,7 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C31" t="s">
@@ -1380,7 +1390,7 @@
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C32" t="s">
@@ -1391,7 +1401,7 @@
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C33" t="s">
@@ -1402,7 +1412,7 @@
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C34" t="s">
@@ -1413,7 +1423,7 @@
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C35" t="s">
@@ -1424,7 +1434,7 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C36" t="s">
@@ -1435,7 +1445,7 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C37" t="s">
@@ -1446,7 +1456,7 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C38" t="s">
@@ -1457,7 +1467,7 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>110</v>
       </c>
       <c r="C39" t="s">
@@ -1468,7 +1478,7 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C40" t="s">
@@ -1479,7 +1489,7 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C41" t="s">
@@ -1490,7 +1500,7 @@
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C42" t="s">
@@ -1501,7 +1511,7 @@
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C43" t="s">
@@ -1512,7 +1522,7 @@
       <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C44" t="s">
@@ -1523,7 +1533,7 @@
       <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>116</v>
       </c>
       <c r="C45" t="s">
@@ -1534,7 +1544,7 @@
       <c r="A46" t="s">
         <v>47</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C46" t="s">
@@ -1545,7 +1555,7 @@
       <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C47" t="s">
@@ -1556,7 +1566,7 @@
       <c r="A48" t="s">
         <v>49</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C48" t="s">
@@ -1567,7 +1577,7 @@
       <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C49" t="s">
@@ -1578,7 +1588,7 @@
       <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C50" t="s">
@@ -1589,7 +1599,7 @@
       <c r="A51" t="s">
         <v>52</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C51" t="s">
@@ -1600,7 +1610,7 @@
       <c r="A52" t="s">
         <v>53</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C52" t="s">
@@ -1611,7 +1621,7 @@
       <c r="A53" t="s">
         <v>54</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C53" t="s">
@@ -1622,7 +1632,7 @@
       <c r="A54" t="s">
         <v>55</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C54" t="s">
@@ -1633,7 +1643,7 @@
       <c r="A55" t="s">
         <v>56</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C55" t="s">
@@ -1644,7 +1654,7 @@
       <c r="A56" t="s">
         <v>57</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C56" t="s">
@@ -1655,7 +1665,7 @@
       <c r="A57" t="s">
         <v>58</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C57" t="s">
@@ -1666,7 +1676,7 @@
       <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C58" t="s">
@@ -1677,7 +1687,7 @@
       <c r="A59" t="s">
         <v>60</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>130</v>
       </c>
       <c r="C59" t="s">
@@ -1688,7 +1698,7 @@
       <c r="A60" t="s">
         <v>61</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C60" t="s">
@@ -1699,7 +1709,7 @@
       <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C61" t="s">
@@ -1710,7 +1720,7 @@
       <c r="A62" t="s">
         <v>63</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C62" t="s">
@@ -1721,7 +1731,7 @@
       <c r="A63" t="s">
         <v>64</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>134</v>
       </c>
       <c r="C63" t="s">
@@ -1732,7 +1742,7 @@
       <c r="A64" t="s">
         <v>65</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C64" t="s">
@@ -1743,7 +1753,7 @@
       <c r="A65" t="s">
         <v>66</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>136</v>
       </c>
       <c r="C65" t="s">
@@ -1754,7 +1764,7 @@
       <c r="A66" t="s">
         <v>67</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C66" t="s">
@@ -1765,7 +1775,7 @@
       <c r="A67" t="s">
         <v>68</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C67" t="s">
@@ -1776,7 +1786,7 @@
       <c r="A68" t="s">
         <v>69</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C68" t="s">
@@ -1787,7 +1797,7 @@
       <c r="A69" t="s">
         <v>70</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C69" t="s">
@@ -1798,7 +1808,7 @@
       <c r="A70" t="s">
         <v>71</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C70" t="s">
@@ -1809,7 +1819,7 @@
       <c r="A71" t="s">
         <v>72</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C71" t="s">
@@ -1818,5 +1828,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>